<commit_message>
Log de pruebas 34
</commit_message>
<xml_diff>
--- a/Sprint#4/Pruebas Individuales/Log pruebas individuales RF-34.xlsx
+++ b/Sprint#4/Pruebas Individuales/Log pruebas individuales RF-34.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivane\OneDrive\Documentos\GitHub\SIGAB\Sprint#3\Pruebas Individuales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivane\OneDrive\Documentos\GitHub\SIGAB\Sprint#4\Pruebas Individuales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B593F8-B7B0-4F3D-8FC2-07C407C7F7C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12496479-853E-45EF-8A52-F033DE46D987}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FF637D33-BA58-4CB0-B19F-1F4A4D7557B5}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FF637D33-BA58-4CB0-B19F-1F4A4D7557B5}"/>
   </bookViews>
   <sheets>
-    <sheet name="RF 22" sheetId="1" r:id="rId1"/>
-    <sheet name="Firmas" sheetId="2" r:id="rId2"/>
+    <sheet name="RF 34" sheetId="1" r:id="rId1"/>
+    <sheet name="Datos de prueba" sheetId="3" r:id="rId2"/>
+    <sheet name="Firmas" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,8 +44,183 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{18BA6529-8903-43C2-9B6C-F50C46D75312}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>======
+ID#AAAAMO-VWSY
+Julate69    (2021-04-24 19:30:49)
+Digitar número de cédula sin guiones, ni espacios</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{062B70A4-107C-42C6-920B-5B111F531594}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>======
+ID#AAAAMO-VWSQ
+Julate69    (2021-04-24 19:30:49)
+Digitar sin guiones, ni espacios</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{1B6C9ECD-864F-4FAE-9ED8-43D4B02A755D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>======
+ID#AAAAMO-VWSE
+Julate69    (2021-04-24 19:30:49)
+Digitar sin guiones, ni espacios</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{BEE99703-55CB-46C2-B63A-2C9C45DB94EC}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>======
+ID#AAAAMO-VWSI
+Julate69    (2021-04-24 19:30:49)
+Puede digitar alguna de las siguientes opciones, según corresponda:
+Categoría 21 (Técnico Auxiliar)
+Categoría 23 (Técnico General 1-2-3)
+Categoría 24 (Técnico Analista 1-2-3)
+Categoría 32 (Profesional Asistencial 1-2-3-4-5)
+Categoría 34 (Profesional Ejecutivo 1-2-3-4)
+Categoría 35 (Profesional Analista 1-2-3)
+Categoría 36 (Profesional Especialista)
+Categoría 37 (Profesional Asesor de Procesos 1-2)
+Categoría 38 (Profesional Asesor General)
+Categoría 42 (Director Ejecutivo)
+Categoría 43 (Director Especialista)
+Categoría 44 (Director Asesor)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{C31E0A57-5BFC-46E3-BE38-C2BE98FC2251}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>======
+ID#AAAAMO-VWSc
+Julate69    (2021-04-24 19:30:49)
+Puede agregar alguna de las siguientes opciones:
+Categoría 87 (Profesor Instructor Bachiller)
+Categoría 88 (Profesor Instructor Licenciado)
+Categoría 89 (Profesor I)
+Categoría 90 (Profesor II) 
+Categoría 91 (Catedrático)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{8A2BFFC5-1C80-456B-9C78-69A58D9BE304}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>======
+ID#AAAAMO-VWSg
+Julate69    (2021-04-24 19:30:49)
+Tiempo completo (40 horas)
+Cuarto de tiempo (30 horas)
+Medio tiempo (30 horas)
+Un cuarto de tiempo (10 horas)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{75C28CE7-6B18-49FC-A1DF-49D79A3C77F8}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>======
+ID#AAAAMO-VWSk
+Julate69    (2021-04-24 19:30:49)
+Digitar alguna de las siguientes opciones:
+Dirección
+Subdirección 
+Profesional Ejecutivo 
+Técnico Auxiliar
+Profesional Asistencial en Desarrollo Tecnológico
+Profesional Ejecutivo en Desarrollo Documental 
+Responsable de PPAA
+Participante de PPAA
+Docente 
+(Si participa en más de una, favor separarlos con punto y coma (;))</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{DB2289A3-1880-4F5E-8308-40D9FE68AF26}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>======
+ID#AAAAMO-VWSU
+Julate69    (2021-04-24 19:30:49)
+Aplica para personal docente interino</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{6432F278-2535-417E-878E-15351DA205BD}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>======
+ID#AAAAMO-VWSM
+Julate69    (2021-04-24 19:30:49)
+Año en el que obtuvo la propiedad en la UNA</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="149">
   <si>
     <t>Observación</t>
   </si>
@@ -77,9 +253,6 @@
   </si>
   <si>
     <t>No cumple</t>
-  </si>
-  <si>
-    <t>Criterios de aceptación definidos en el RF 1 (AZURE)</t>
   </si>
   <si>
     <t>Log de pruebas individuales (comprobación de criterios de aceptación)</t>
@@ -99,26 +272,471 @@
     <t>X</t>
   </si>
   <si>
-    <t>No aplica</t>
-  </si>
-  <si>
-    <t>Visualizar documentos de evidencia de una actividad</t>
-  </si>
-  <si>
-    <t>Las evidencias se observan mediante una opción en el detalle de cada actividad.</t>
-  </si>
-  <si>
-    <t>En caso de que no se pueda mostrar una previsualización se puede descargar el documento.</t>
-  </si>
-  <si>
-    <t>En caso de ser un vídeo de Youtube se mostrará el link de reedireción.</t>
+    <t>Generar datos y estadísticas acerca del involucramiento del personal</t>
+  </si>
+  <si>
+    <t>Una consulta sobre el porcentaje de participación del personal (del año en curso) en las diferentes actividades según el tipo.
+Una consulta sobre el porcentaje de participación del personal (del año en curso) en las diferentes actividades según el ámbito (Nacional o Internacional).</t>
+  </si>
+  <si>
+    <t>Realizar la consulta de información de participación de un personal en específico. Para dicha consulta se seguirán los siguientes parámetros:
+Cédula del personal. 
+Rango de fechas. 
+Estado de la actividad.</t>
+  </si>
+  <si>
+    <t>Los gráficos generados por dicha consulta serán los siguientes: 
+Participación en diferentes actividades por tipos. En el gráfico se mostrarán los tipos de actividades y el número de actividades en las que participó en ese rango de fechas y con el estado seleccionado. Este gráfico será de tipo “Gráfico de Dona”. 
+Cantidad de participación por fechas. En el eje “X” se mostrarán los meses y en eje “Y” el número de actividades en las que participó. Este gráfico será de tipo “Gráfico de Área”. 
+Participación en actividades por ámbito. En el eje “X” se mostrarán los siguientes valores: “Internacional”, “Nacional”, y en el eje “Y” se mostrarán el número de actividades en las que participó en ese rango de fechas y con el estado seleccionado. Este gráfico será de tipo “Gráfico de Barras”.</t>
+  </si>
+  <si>
+    <t>Se encuentra en las hoja de datos de prueba</t>
+  </si>
+  <si>
+    <t>Criterios de aceptación definidos en el RF 34 (AZURE)</t>
+  </si>
+  <si>
+    <t>ID (*)</t>
+  </si>
+  <si>
+    <t>Nombre (*)</t>
+  </si>
+  <si>
+    <t>Apellidos (*)</t>
+  </si>
+  <si>
+    <t>Fecha 
+nacimiento (*)</t>
+  </si>
+  <si>
+    <t>Género (*)</t>
+  </si>
+  <si>
+    <t>Correo 
+personal</t>
+  </si>
+  <si>
+    <t>Correo 
+institucional (*)</t>
+  </si>
+  <si>
+    <t>Teléfono 
+fijo</t>
+  </si>
+  <si>
+    <t>Teléfono 
+celular</t>
+  </si>
+  <si>
+    <t>Estado civil (*)</t>
+  </si>
+  <si>
+    <t>Dirección 
+residencia (*)</t>
+  </si>
+  <si>
+    <t>Grado académico (*)</t>
+  </si>
+  <si>
+    <t>Área de especialización (puede indicar hasta 2 áreas de especialización separándolas por punto y coma (;))</t>
+  </si>
+  <si>
+    <t>Tipo de nombramiento (*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Régimen 
+administrativo
+</t>
+  </si>
+  <si>
+    <t>Regimen docente</t>
+  </si>
+  <si>
+    <t>Jornada laboral (*)</t>
+  </si>
+  <si>
+    <t>Cargo (*)</t>
+  </si>
+  <si>
+    <t>Tipo de puesto (*)</t>
+  </si>
+  <si>
+    <t>Lugar trabajo externo</t>
+  </si>
+  <si>
+    <t>Año propiedad (*)</t>
+  </si>
+  <si>
+    <t>Carga académica 
+(separar cada curso con punto y coma (;))</t>
+  </si>
+  <si>
+    <t>Experiencia profesional 
+(separar cada "ocurrencia" con punto y coma (;))</t>
+  </si>
+  <si>
+    <t>Experiencia académica 
+(separar cada curso con punto y coma (;))</t>
+  </si>
+  <si>
+    <t>Capacitación didáctica 
+(separar cada curso con punto y coma (;))</t>
+  </si>
+  <si>
+    <t>Publicaciones 
+(separar cada publicación con punto y coma (;))</t>
+  </si>
+  <si>
+    <t>Idiomas 
+(Indicar los nombres de los idiomas que maneja) 
+(separar cada idioma con punto y coma (;))</t>
+  </si>
+  <si>
+    <t>Miembro comisiones 
+(separar cada uno con punto y coma (;))</t>
+  </si>
+  <si>
+    <t>Tutorias 
+(separar cada tutoría con punto y coma (;))</t>
+  </si>
+  <si>
+    <t>Lectorías 
+(separar cada lectoría con punto y coma (;))</t>
+  </si>
+  <si>
+    <t>Miembro pruebas de grado 
+(separar cada prueba de grado en la que ha participado con punto y coma (;))</t>
+  </si>
+  <si>
+    <t>Evaluador (Tribunal defensas públicas)
+(separar cada evaluación con punto y coma (;))</t>
+  </si>
+  <si>
+    <t>Evaluación interna de PPAA
+(separar cada evaluación con punto y coma (;))</t>
+  </si>
+  <si>
+    <t>Evaluación externa
+PPAA
+(separar cada evaluación con punto y coma (;))</t>
+  </si>
+  <si>
+    <t>Reconocimientos
+(separar cada reconocimiento con punto y coma (;))</t>
+  </si>
+  <si>
+    <t>Jenny</t>
+  </si>
+  <si>
+    <t>Ulate Montero</t>
+  </si>
+  <si>
+    <t>Femenino</t>
+  </si>
+  <si>
+    <t>jmontero692010@hotmail.com</t>
+  </si>
+  <si>
+    <t>jenny.ulate.montero@una.ac.cr</t>
+  </si>
+  <si>
+    <t>Soltera</t>
+  </si>
+  <si>
+    <t>San Pedro de Barva, Heredia, 600 m este de la Iglesia Católica</t>
+  </si>
+  <si>
+    <t>Maestría</t>
+  </si>
+  <si>
+    <t>Tratamiento de la Información</t>
+  </si>
+  <si>
+    <t>Propietaria</t>
+  </si>
+  <si>
+    <t>Categoría 88 (Profesor Instructor Licenciado)</t>
+  </si>
+  <si>
+    <t>Tiempo completo</t>
+  </si>
+  <si>
+    <t>Académico</t>
+  </si>
+  <si>
+    <t>Docente;Participante de PPAA</t>
+  </si>
+  <si>
+    <t>Indización y resúmenes;Organización de la Información I;Organización de la Información II;Almacenamiento I;Almacenamiento II; Almacenamiento III;Procesamiento de materiales especiales;Usuarios de la Información;Diseño de Servicios de Información</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asistente del Área de Circulación y Préstamo;Encargada de la Biblioteca Municipal Rafael A. Calderon Guardia;Encargada Centro Catalográfico (Bibliotecas Municipales)
+</t>
+  </si>
+  <si>
+    <t>Tutora en la UNED;Docente en el 2010 de Escuela de Bibliotecología de la Universidad de Costa Rica;Docente de la Escuela de Bibliotecología de la Universidad Nacional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planificación para los aprendizajes significativos en la Universidad Nacional (2019);Pedagogía Universitaria para la Educación a Distancia (2015);Organización y diseño de cursos en línea (2015);Mediación pedagógica para el aprendizaje con sentido (2017);Evaluación de los Aprendizajes significativos en la universidad (2018);Curso-Taller para la integración de las TICS en los cursos universitarios (2019)
+Diseño pedagógico, mediación pedagógica y evaluación para los aprendizajes en programas de curso con modalidades virtuales (2019)
+</t>
+  </si>
+  <si>
+    <t>Ulate Montero J. (2020). Propuesta de un Sistema Integrado de Gestión Bibliotecaria para el Sistema de Bibliotecas Municipales de la Municipalidad de San Jose.
+Bibliotecas, 38, (1), pp. 1-27.</t>
+  </si>
+  <si>
+    <t>Manejo instrumental del Inglés</t>
+  </si>
+  <si>
+    <t>Miembro de la Comisión Diseño Curricular</t>
+  </si>
+  <si>
+    <t>Lectora del Trabajo Final de Graduación: Control documental sobre bioluminiscencia en Costa Rica: 1900-2018</t>
+  </si>
+  <si>
+    <t>Organización de la información;Desarrollo de Colección;Servicios de información virtuales</t>
+  </si>
+  <si>
+    <t>Nombre del proyecto académico:  Diseño de una unidad didáctica para el uso de las RDA (Descripción y Acceso de Recursos)</t>
+  </si>
+  <si>
+    <t>Graduación de honor en el 2018 del Programa de Posgrado en Bibliotecología y Estudios de la Información</t>
+  </si>
+  <si>
+    <t>Lucrecia</t>
+  </si>
+  <si>
+    <t>Barboza Jiménez</t>
+  </si>
+  <si>
+    <t>lucreciabj@hotmail.com</t>
+  </si>
+  <si>
+    <t>lucrecia.barboza.jimenez@una.ac.cr</t>
+  </si>
+  <si>
+    <t>Aserrí centro, 50 m sur del Banco Nacional, carretera a Cinco Esquinas</t>
+  </si>
+  <si>
+    <t>Investigación;Conservación y preservación de materiales</t>
+  </si>
+  <si>
+    <t>Categoría 90 (Profesor II)</t>
+  </si>
+  <si>
+    <t>Docente;Responsable de PPAA;Participante de PPAA</t>
+  </si>
+  <si>
+    <t>Control documental nacional e internacional;Indización y resúmenes;Gestión para el conocimiento;Liderazgo y recursos humanos;Investigación I;InvestigaciónII;  Introducción a la Bibliotecología y Documentación;Documentación; Desarrollo de colecciones;Conservación y preservación de materiales documentales; Patrimonio documental y su preservación;Debates epistemológicos de la Bibliotecología</t>
+  </si>
+  <si>
+    <t>Asistente en la Biblioteca de Ciencias Sociales (UCR);Asistente en la Biblioteca Asociación de Colegios del Medio Oeste (ACM);Asistente en la Biblioteca del Centro de Investigaciones en Tecnología de Alimentos (UCR);Bibliotecóloga de la Asociación Demográfica Costarricense;Encargada de biblioteca del Instituto Dr. Jaim Weizman;Encargada de Biblioteca del Colegio Internacional SOS Hermann Gmeiner;Bibliotecóloga del Proyecto Automatización del Centro de Documentación del Instituto Costarricense de Acueductos y Alcantarillados (AyA);Técnico asistente de la Biblioteca José Figueres Ferrer (ITCR);Encargada de biblioteca Escuela Libre de Derecho;Contrato laboral con la Biblioteca de Ciencias Sociales (UCR)</t>
+  </si>
+  <si>
+    <t>Académica de la Escuela dee Bibliotecología, Documentación e Información de la Universidad Nacional desde el 2006</t>
+  </si>
+  <si>
+    <t>Curso/taller: Estrategias para potenciar el trabajo colaborativo como herramienta en la mediación pedagógica; Curso/taller: Estrategias para potenciar el pensamiento crítico y creativo en los procesos de mediación; Curso Planificación para los aprendizajes significativos en la universidad; Curso-taller Integración de las TIC en cursos universitarios; Curso Evaluación para los aprendizajes significativos en la universidad; Curso Mediación pedagógica para el aprendizaje con sentido; Taller Inducción a los procesos de autoevaluación en el marco de la gestión de calidad; Taller Internacionalización del currículum; Taller Guía académico; Curso Gestión pública en instancias académicas; Taller buenas prácticas docentes; Curso Diseño pedagógico y metodológico de cursos universitarios en modalidad virtual o bimodal; Taller Propiedad intelectual aplicado a la integración de tecnología en educación en cursos presenciales bimodales y virtuales; Curso Educación emocional para académicos; Módulo Modelo de capacitación para analistas del informe de autoevaluación; Curso Portafolio electrónico como apoyo al proceso de aprendizaje; Curso Promoción de los aprendizajes en la docencia universitaria; Taller Inducción a la vida universitaria</t>
+  </si>
+  <si>
+    <t>Azofeifa Mora, Ana Beatriz, Barboza Jiménez, Lucrecia, Calvo Sánchez, Loireth, Rojas Morales, Nidia, Solano López, Eduardo. (2015). Informe de autoevaluación de la carrera de Licenciatura y Bachillerato en Bibliotecología y Documentación con salida lateral de Diplomado. Heredia, C.R.: Escuela de Bibliotecología, Documentación e Información; Barboza Jiménez, Lucrecia. (2013). Análisis de la colección de la Sala de Libros Antiguos y Especiales (SLAE) de la Universidad Nacional, Costa Rica y propuesta de directrices para su organización, procesamiento, conservación, preservación y difusión. (Tesis de maestría inédita). Universidad Nacional, Heredia, Costa Rica; Barboza Jiménez, Lucrecia. (2008). Autoevaluación de Diplomado, Bachillerato y Licenciatura en Bibliotecología y Documentación (Empleadores).  Heredia, CR.: Escuela de Bibliotecología, Documentación e Información; Barboza Jiménez, Lucrecia. (2008). Autoevaluación de Diplomado, Bachillerato y Licenciatura en Bibliotecología y Documentación (Estudiantes Primer Ingreso).  Heredia, CR.: Escuela de Bibliotecología, Documentación e Información; Barboza Jiménez, Lucrecia. (2008). Autoevaluación de Diplomado, Bachillerato y Licenciatura en Bibliotecología y Documentación (Estudiantes Regulares).  Heredia, CR.: Escuela de Bibliotecología, Documentación e Información; Barboza Jiménez, Lucrecia. (2014). Educación e investigación en Bibliotecología: caso Universidad Nacional, Costa Rica. Ponencia presentada en el Seminario Iberoamericano sobre Desarrollo Disciplinar en Ciencias Bibliotecológicas y de la Información, 26, 27 y 28 noviembre, San José, Costa Rica; Barboza Jiménez, Lucrecia. (2008). Estudio de usuarios de las comunidades Jardines 1 y Jardines 2 que atiende la biblioteca infantil “Miriam Álvarez Brenes”. Heredia, C.R.: Escuela de Bibliotecología, Documentación e Información; Barboza Jiménez, Lucrecia. (2008). Estudio de usuarios de las comunidades Jardines 1 y Jardines 2 que atiende la biblioteca infantil “Miriam Álvarez Brenes”. Bibliotecas 26 (2): 5-35. Disponible en: http://www.revistas.una.ac.cr/index.php/bibliotecas/article/view/237;</t>
+  </si>
+  <si>
+    <t>Miembro del Consejo de Unidad Académica;Comisión de Trabajos Finales de Graduación</t>
+  </si>
+  <si>
+    <t>Propuesta de servicios de información para niños y niñas con necesidades educativas especiales del Centro de Enseñanza Especial de Heredia (2017); Propuesta de servicios de información para el centro de documentación de la Facultad de Educación de la Universidad de Costa Rica para transformarlo en biblioteca universitaria en ciencias de la educación (2016); Integración de la biblioteca de la Escuela La Trinidad al currículo escolar y a la comunidad educativa (2015); Propuesta para la integración de la biblioteca al currículo escolar de la Escuela Manuel Camacho Hernández (2014); Propuesta para la integración de la biblioteca escolar al currículo educativo de la Escuela 12 de Marzo de 1948, circuito 01, Dirección Regional de Educación Pérez Zeledón (2014); Propuesta para la integración efectiva entre la biblioteca y la comunidad educativa con respecto a la aplicabilidad del currículo en la Escuela Pedro Pérez Zeledón (2014); Propuesta para la integración efectiva de la Biblioteca del Liceo Las Mercedes con Orientación Tecnológica, circuito 06, Región Educativa Pérez Zeledón, Costa Rica, al currículo escolar (2014); Propuesta para la integración efectiva del Centro de Recursos para el Aprendizaje de la Escuela Sinaí, Pérez Zeledón, Costa Rica, al currículo educativo (2014); La integración efectiva entre la Escuela La Aurora, Heredia, Costa Rica, y su biblioteca: un espacio de aprendizaje”, comunica que mi persona ya ha hecho las observaciones necesarias a dicha investigación y al igual que las sugeridas por los lectores ya fueron incorporadas por las estudiantes (2014); Integración de la biblioteca de la Escuela Elisa Soto Jiménez, Heredia, Costa Rica, al currículo escolar y a la comunidad educativa (2014); La biblioteca escolar de la institución Hernán Rodríguez Ruíz del distrito Daniel Flores de Pérez Zeledón y su integración efectiva al currículo y a la comunidad educativa (2014)</t>
+  </si>
+  <si>
+    <t>Sistema para la organización, recuperación y difusión de la información de los expedientes sobre daños al ambiente tramitados por el Tribunal Ambiental Administrativo de Costa Rica (2015); Análisis bibliométrico de la producción científica de la Revista Geográfica de América Central en los años 1974-2010 y su uso en los trabajos finales de graduación y los programas de cursos de la Escuela de Ciencias Geográficas de la Universidad Nacional de Costa Rica (UNA) (2014); Propuesta de servicios especiales para la Biblioteca Municipal Carmen Lyra, a partir del análisis de la comunidad de Rincón Grande de Pavas (2013); Propuesta para la creación de repositorios digitales sobre la producción intelectual institucional, aplicando la experiencia en cuatro instituciones públicas costarricenses: Subgerencia de Ambiente, Investigación y Desarrollo del Instituto Costarricense de Acueductos y Alcantarillados (AyA), Centro de Gestión Ambiental de la Unidad Estratégica de Negocios de Proyectos y Servicios Asociados (UEN-PySA) del Instituto Costarricense de Electricidad (ICE), Oficina de Relaciones Públicas de la Universidad Nacional y Consejo Nacional de Rehabilitación y Educación Especial (2013)</t>
+  </si>
+  <si>
+    <t>Docente distinguida 2008 por la Escuela de Bibliotecología, Documentación e Información; Participante en la publicación del libro “La evaluación de la educación bibliotecológica en América Latina” 2011; Docente exitoso de la Universidad Nacional (evaluación del desempeño docente excelente de 2008 – 2013)</t>
+  </si>
+  <si>
+    <t>Loireth</t>
+  </si>
+  <si>
+    <t>Calvo Sánchez</t>
+  </si>
+  <si>
+    <t>loirethc@gmail.com</t>
+  </si>
+  <si>
+    <t>loirette.calvo.sanchez@una.ac.cr</t>
+  </si>
+  <si>
+    <t>Casada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">San Antonio de Belén, Urbanización Veredas del Río. Casa número 30 </t>
+  </si>
+  <si>
+    <t>Docente;Responsable de PPA</t>
+  </si>
+  <si>
+    <t>Taller de investigación II;Proyecto de investigación</t>
+  </si>
+  <si>
+    <t>Bibliotecologa (Centro de Documentación del IIDH);Consulturía (automatización del archivo vertical Biblioteca Pública de Belén );Encargada del área de Catalogación (Biblioteca Corte Interamericana de Derechos Humanos)</t>
+  </si>
+  <si>
+    <t>Académica de Escuela de Bibliotecología de la Universidad Nacional; Docente Escuela de Bibliotecología Universidad de Costa Rica</t>
+  </si>
+  <si>
+    <t>Planificación para los aprendizajes significativos en la Universidad Nacional (2019);Pedagogía Universitaria para la Educación a Distancia (2015);Organización y diseño de cursos en línea (2015);Mediación pedagógica para el aprendizaje con sentido (2017);Evaluación de los Aprendizajes significativos en la universidad (2018);Curso-Taller para la integración de las TICS en los cursos universitarios (2019)
+Diseño pedagógico, mediación pedagógica y evaluación para los aprendizajes en programas de curso con modalidades virtuales (2019)</t>
+  </si>
+  <si>
+    <t>Calvo Sánchez, L. (2020). Experiencia metodológica utilizada por las docentes de la Escuela de Bibliotecología, Documentación e Información en la incorporación de RDA en los programas de curso. Bibliotecas, 38(1), 1 – 22;  Calvo Sánchez, L. (2018). Los Juegos cooperativos y el acceso a la información desde la extensión Universitaria Revista E-Ciencias de la información 8 (1)1-19;  Calvo Sánchez, L. (2017). Marc 21 bibliografico y los lenguajes documentales: San José, Costa Rica : Editorial de la Universidad de Costa Rica ; Calvo Sánchez, L. (2017). Los Requisitos Funcionales de los Registros Bibliográficos (FRBR), su relación con las RDA y los cambios que se avecinan. Bibliotecas, 35(1), 1-22.; Calvo Sánchez, L. (2015). Desarrollo de guías didácticas con herramientas colaborativas para cursos de bibliotecología y ciencias de la información. Revista E-Ciencias de la información 5 (1)1-19 ;  Calvo Sánchez, L (2000). Manual de Procedimientos para la Prestación de los Servicios. San José, Costa Rica : Corte Interamericana de Derechos Humanos;  Molina, L., Calvo, L. (1999).  Directorio de Organizaciones de Derechos Humanos de Centroamérica y Panamá.  San José, CR. Instituto  Interamericano de Derechos Humanos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manejo Intrumental del Inglés </t>
+  </si>
+  <si>
+    <t>Miembro de la Comisión de Desarrollo Curricular;Comisión de Trabajos Finales de Gradaución;Comisión reconocimento de Atestados;Comisión Evaluadora del concursos por oposición</t>
+  </si>
+  <si>
+    <t>Control documental del cantón de Santo Domingo de Heredia: 1902-2006 (2015)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bibliografía nacional retrospectiva de Costa Rica para la Biblioteca Nacional Miguel Obregón Lizano, correspondiente a los años 1984 y 1985</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve"> (2018)</t>
+    </r>
+  </si>
+  <si>
+    <t>Servicios  de información virtuales;Organización de la información; Arquitectura de Infromación; Servicios de información virtuales</t>
+  </si>
+  <si>
+    <t>Nombre de la actividad Académica : SIGAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freddy </t>
+  </si>
+  <si>
+    <t>Oviedo González</t>
+  </si>
+  <si>
+    <t>Masculino</t>
+  </si>
+  <si>
+    <t>foviedog@gmail.com</t>
+  </si>
+  <si>
+    <t>foviedo@una.ac.cr</t>
+  </si>
+  <si>
+    <t>Casado</t>
+  </si>
+  <si>
+    <t>Santa Lucía de Barva, Heredia. Del consultorio del Dr.Naranjo 200 metros Este y 25 metros Sur.</t>
+  </si>
+  <si>
+    <t>Tecnología e Innovación educativa</t>
+  </si>
+  <si>
+    <t>Propietario</t>
+  </si>
+  <si>
+    <t>Categoria 32 (Profesional Asistencial en Desarrollo Tecnológico)</t>
+  </si>
+  <si>
+    <t>Administrativo</t>
+  </si>
+  <si>
+    <t>Profesional Asistencial en Desarrollo Tecnológico</t>
+  </si>
+  <si>
+    <t>Instituto de Capacitación y Asesoría en Informática (ICAI) de la Universidad Nacional, Cargo Instructor de cursos de capacitación Diseño de páginas Web nivel principiante, 2004-2005, Paquete completo Web (Nivel I, II y III) 2007; Universidad Nacional, Decanato de la Facultad de Filosofía y Letras, 2004 al 2008, cargo: Profesor Instructor Bachiller; Participación en el proyecto de la Colección Bibliográfica Electrónica de la Escuela de Filosofía de la Universidad Nacional; Apoyo Informático y administrativo a las Unidades Académicas de la Facultad de Filosofía y Letras, soporte técnico, mantenimiento de equipos, Instalación y desarrollo de software; Profesional Asistencial en Desarrollo Tecnológico Del 2008 a la fecha.</t>
+  </si>
+  <si>
+    <t>Periodo laborado: 2006 al 2014 Cursos impartidos en la Escuela de Bibliotecología, Documentación e Información, de la Universidad Nacional: Gestión de Recursos Tecnológicos;        Proyectos Tecnológicos; Teoría de Sistemas; Metodologías y Prácticas de Tecnologías de la Información y la Comunicación; Gestión de Tecnología de la Información y Comunicación; Sistemas Colaborativos para educación (Licenciatura en Bibliotecología pedagógica); Unidades de Información Documental Virtuales; Sistemas Colaborativos (Bachillerato en Bibliotecología y Documentación).</t>
+  </si>
+  <si>
+    <t>Bases para el disño de archivos digitales sonoros, Universidad Nacional (2018); Producción de videos educativos, Universidad Nacional (2018); Herramientas en línea para el trabajo colaborativo (2018); Diseño pdagógico y metodológico de cursos virtuales y bimodales (2018); Curso de inglés conversacional
+Curso de Microsoft Excel(2019); Capacitación sobre herramientas para hacer evaluaciones en línea; Taller producción audiovisual (2018 ); Capacitación sobre Aula Virtual(2019) Capacitación sobre Microsoft TEAMS(2020).</t>
+  </si>
+  <si>
+    <t>Oviedo González, F. (2012), Arquetipos bibliotecarios: diseño de una propuesta didáctica multimedia que contribuya con la mejora de la imagen de la bibliotecología en la sociedad costarricense, Revista Bibliotecas Vol. 30, No. 1ene.-jun., 2012. Disponible en: http://www.revistas.una.ac.cr/index.php/bibliotecas/article/view/3891;
+Oviedo González Freddy. (2014), El uso de las TIC en la carrera de Bibliotecología y Documentación, Revista Bibliotecas Vol. 32, No. 2 jul-dic., 2014 pp.16-31. Disponible en: http://www.revistas.una.ac.cr/index.php/bibliotecas/article/view/6457; Oviedo González Freddy. Zúñiga Benavides José F. (2015), Experiencia en la incorporación de recursos web en la plataforma educativa de la Universidad Nacional, Memoria del IV Foro de Innovación Académica. 2015. pp.279-287. Disponible en: http://www.fai.una.ac.cr/images/Memoria.pdf</t>
+  </si>
+  <si>
+    <t>Miembro de la Comisión para atención de emergencias en la FFL</t>
+  </si>
+  <si>
+    <t>Rodríguez, N. (2014). Evaluación de la accesibilidad a la información de las personas con discapacidad visual en los Sitios Web de los Ministerios de Costa Rica.: Universidad Nacional;Peña, L., (2016). Evaluación de Bibliotecas Digitales, Electrónicas y Virtuales Universitarias de Iberoamérica. Heredia, C. R.: Universidad Nacional.</t>
+  </si>
+  <si>
+    <t>Cambronero, D., Fonseca, J., Zamora, K &amp; Zuñiga, D. (2014). La integración efectiva entre la Escuela La Aurora, Herdia, Costa Rica, y su biblioteca: un espacio de aprendizaje.: Universidad Nacional; Cruz, A., (2014) Repositorio de las publicaciones técnico-científicas en la comunidad de practica sobre el enfoque ecosistemico en salud Humana - América Latina y el Caribe, Instituto regional de Estudios en sustancias toxicas, Universidad Nación; Guerrero, G., Mesén, K &amp; Rojas, C. (2014). Propuesta de un plan de promoción y divulgación
+para las bibliotecas públicas de la provincia de Heredia aplicando tecnologías de la información y comunicación. Heredia, C. R.: Universidad Nacional; Tinoco, A., (2016). Tutoriales virtuales para el uso de las bases de datos Annual Reviews,
+EBSCO y ProQuest para la comunidad Universitaria de la Sede Interuniversitaria de Alajuela compuesta por estudiantes de la Universidad de Costa Rica, el Instituto Tecnológico de Costa Rica, la Universidad Nacional y la Universidad Estatal a Distancia. Heredia, C. R.: Universidad Nacional; Chanto, E &amp; Arroyo, T. (2017). Evaluación de los documentos impresos de las áreas de obras generales (000), Ciencias Sociales, Ciencias políticas (300), Lenguaje, lingüística (400) Ciencias Puras (500), Ciencias aplicadas (600) de la Biblioteca Luis Ferrero Acosta de la Sede del pacífico de la Universidad de Costa Rica.: Universidad Nacional; Navarro, E (2019). Repositorio de Trabajos Finales de Graduación de la Universidad Central, Aprobados durante los años comprendidos del 2014 al 2016.</t>
+  </si>
+  <si>
+    <t>Tecnologías de la Información y de la Comunicación</t>
+  </si>
+  <si>
+    <t>Mejor promedio de posgrados 2011; Estudiante distinguido 2011 de la Maestría en Tecnología e Informática Educativa; Mención CUM LAUDE en la Maestría en Tecnología e Informática Educativa; Docente exitoso de la Universidad Nacional (evaluación del desempeño docente excelente de 2008 – 2013); Docente exitoso de la Universidad Nacional (período 2013-2014) Universidad Nacional.</t>
+  </si>
+  <si>
+    <t>Ana Magally</t>
+  </si>
+  <si>
+    <t>Campos Méndez</t>
+  </si>
+  <si>
+    <t>magally.campos.mendez@una.cr</t>
+  </si>
+  <si>
+    <t>Heredia. Urbanización Monte Rosa. Casa 176 E</t>
+  </si>
+  <si>
+    <t>Administración de Proyectos Informáticos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operadora de Computadoras. Universidad Nacional Períodos de Matrícula Departamento de Registro;Operadora de Computadoras. Constructora Edificadora Roma Departamento de Contabilidad;Asistente Académico 1.Laboratorio de Oceanografía y Manejo Costero (LAOCOS). Universidad Nacional Procesamiento de Imágenes;Administradora de Novell 3.11. Laboratorio de Informática. Soporte de la Red Novell. Universidad Nacional;Administradora de Novell 4.10. Laboratorio de Informática. Soporte de la Red Novell. Universidad Nacional. Instalación y Mantenimiento de la Red Administración General (Usuarios, Seguridad etc.);Asistente Académico. Laboratorio Informática/Matemática. Soporte, mantenimiento de máquinas e instalación de programas. Universidad Nacional;Técnico2 en Informática. Centro de Cómputo. Capacitación Developer/2000 (Form Builder y Report Builder), Capacitación en Oracle9i Designer, Administradora de los Servidores de Imágenes y Archivos Proceso de Digitalización Universidad Nacional;Profesional Asistencial en Desarrollo Tecnológico. Escuela de Bibliotecología, Documentación e Información.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Académica Curso de Teoría de Sistemas. BGE418. Escuela de Bibliotecología, Documentación e Información;Académica Curso Sistemas Colaborativos. BGE421. Escuela de Bibliotecología, Documentación e Información;Académica Curso Teoría de Sistemas BGE418 IV Nivel Tutoría. Escuela de Bibliotecología, Documentación e Información;Académica Curso Sistemas de Información. Nivel Licenciatura. Escuela de Bibliotecología, Documentación e Información;Lectora de la tesis denominada “Repositorio de las publicaciones técnico científicas en la comunidad de práctica sobre el enfoque ecosistémico en salud humana –América latina y el Caribe, Instituto Regional de Estudios en Sustancias Tóxicas, Universidad Nacional”;Lectora de la Tesis denominada “Repositorio de trabajos finales de graduación de la Universidad Central aprobados durante los años comprendidos del 2014 al 2016, Universidad Nacional.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modelo y Diseño de Base de Datos, 08/11/1998 Oficentro Ejecutivo de Oracle;Introduccion a Oracle: SQL/PL/SQL utilizando Procedure Builder, 15/06/1998 al 26/06/1998 Oficentro Ejecutivo de Oracle;Developer /2000:Reports 2.5, 15 /07/1998 al 22/07/1998, Oficentro Ejecutivo de Oracle; Developer/2000: Forms 4.5 I Parte, 01/07/1998 al 14/07/1998, Oficentro Ejecutivo de Oracle; Modelo y Diseño de Bases de Datos, 12/07/1999 al 13/07/1999 Oficentro Ejecutivo de Oracle;Introduccion a Oracle: Sql y PL/SQL utilizando Procedure Builder, 14/07/1999 al 20/07/1999, Oficentro Ejecutivo de Oracle; Developer/2000: Build Reports, 28/07/1999 al 30/07/1999, Oficentro Ejecutivo de Oracle;Aplication Development 2, Enero 2000, Oficentro Ejecutivo Oracle;Power Builder Version 7.0, 05/08/2002 al 26/08/2002, Universidad Nacional;Oracle 9i Designer: Forms Design and Generation, 17/02/2003 al 21/02/2003, Oficentro Ejecutivo de Oracle;Pedagogia Universitaria, 29/08/2005 al 07/12/2005, Universidad Nacional;Flash Nivel I, 25/01/2007 al 22/03/2007, Universidad Nacional;Flash Nivel II, 29/03/2007 al 31/05/2007, Universidad Nacional;Introducción a la Informática basado en Software Libre, 24/11/2008 al 12/12/2008, Universidad Nacional;Programación PHP, 24 y 31 de octubre, 7, 14 y 21 de noviembre de 2009, Universidad Nacional;Manejo Instrumental del Inglés, 27/09/2012, Universidad Nacional; Curso Desarrollo de Habilidades Pedagógicas y Técnicas en el uso de las  Pizarras Digitales Interactivas, 06,13,20 y 27 de mayo de 2014;Curso Desarrollo de habilidades pedagógicas y técnicas en el uso PDI, julio del 2014. Universidad Nacional; Curso Uso de Herramientas Avanzadas del Aula Virtual: Videoconferencias, 04/02/2015, Universidad Nacional;Redacción de documentos. 01/03/2016 al 26/04/2016. Universidad Nacional
+</t>
+  </si>
+  <si>
+    <t>Miranda, G. y Campos, M. (2013). Integración de tecnología y pedagogía en la Biblioteca Infantil “Miriam Álvarez Brenes” de la Universidad Nacional. Bibliotecas. 31(1)Recuperado de: http://www.revistas.una.ac.cr/index.php/bibliotecas/article/view/5107;Campos, M. (2013). La mediación pedagógica en el uso de las tecnologías de la comunicación e información en la Biblioteca Infantil Miriam Álvarez Brenes y la comunidad indígena de Salitre. Bibliotecas. 3(2) Recuperado de: http://www.revistas.una.ac.cr/index.php/bibliotecas/article/view/5887</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repositorio de las publicaciones técnico científicas en la comunidad de práctica sobre el enfoque ecosistémico en salud humana –América latina y el Caribe, Instituto Regional de Estudios en Sustancias Tóxicas, Universidad Nacional  (2014);Repositorio de trabajos finales de graduación de la Universidad Central aprobados durante los años comprendidos del 2014 al 2016, Universidad Nacional.(2020)
+</t>
+  </si>
+  <si>
+    <t>Docente Exitoso en la Universidad Nacional Período 2013-2014. 15 de abril del 2015</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,8 +804,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,8 +858,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -227,12 +873,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -280,6 +941,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -297,72 +1003,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>136</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3180F6CE-C01B-46D5-A8D8-0C7444A26D2E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="15182850" cy="26022300"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -678,16 +1318,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FDCFA43-D090-4464-8DFA-848ABAD3AE83}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.28515625" customWidth="1"/>
+    <col min="1" max="1" width="72.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="47" customWidth="1"/>
+    <col min="5" max="5" width="62.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -702,7 +1342,7 @@
     </row>
     <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -718,7 +1358,7 @@
         <v>18</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
@@ -729,7 +1369,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -741,10 +1381,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="12">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
@@ -755,7 +1395,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
@@ -791,10 +1431,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>10</v>
@@ -806,30 +1446,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" ht="239.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="B13" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -843,7 +1483,7 @@
     </row>
     <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -901,14 +1541,619 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0E8E67-46EA-4C34-A353-154B393A1644}">
+  <dimension ref="A1:AI6"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:AI6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:35" ht="195" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="T1" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="U1" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="V1" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="W1" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="X1" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y1" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z1" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA1" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB1" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC1" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD1" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE1" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF1" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG1" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH1" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI1" s="21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="22">
+        <v>401500844</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="23">
+        <v>25509</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="22">
+        <v>22372096</v>
+      </c>
+      <c r="I2" s="22">
+        <v>89986757</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="N2" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="O2" s="22"/>
+      <c r="P2" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q2" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="R2" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="S2" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22">
+        <v>2019</v>
+      </c>
+      <c r="V2" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="W2" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="X2" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y2" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z2" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA2" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB2" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC2" s="22"/>
+      <c r="AD2" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE2" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF2" s="26"/>
+      <c r="AG2" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH2" s="22"/>
+      <c r="AI2" s="26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="22">
+        <v>107090236</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="23">
+        <v>24770</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22">
+        <v>83666946</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="K3" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="L3" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="M3" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="N3" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q3" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="R3" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="S3" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22">
+        <v>2015</v>
+      </c>
+      <c r="V3" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="W3" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="X3" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y3" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z3" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA3" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB3" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="AC3" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD3" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE3" s="30"/>
+      <c r="AF3" s="22"/>
+      <c r="AG3" s="22"/>
+      <c r="AH3" s="22"/>
+      <c r="AI3" s="25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="22">
+        <v>204770946</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="23">
+        <v>26273</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" s="22">
+        <v>22393615</v>
+      </c>
+      <c r="I4" s="22">
+        <v>83624159</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="K4" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="L4" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="M4" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="O4" s="22"/>
+      <c r="P4" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q4" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="R4" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="S4" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22">
+        <v>2016</v>
+      </c>
+      <c r="V4" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="W4" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="X4" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y4" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z4" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA4" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB4" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC4" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD4" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE4" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF4" s="22"/>
+      <c r="AG4" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH4" s="22"/>
+      <c r="AI4" s="22"/>
+    </row>
+    <row r="5" spans="1:35" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="22">
+        <v>110770945</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="23">
+        <v>29460</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H5" s="22">
+        <v>25624243</v>
+      </c>
+      <c r="I5" s="22">
+        <v>88110706</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="K5" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="L5" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="M5" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="N5" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="O5" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="R5" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="S5" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="T5" s="31"/>
+      <c r="U5" s="22">
+        <v>2015</v>
+      </c>
+      <c r="V5" s="32"/>
+      <c r="W5" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="X5" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y5" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z5" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA5" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB5" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="AC5" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="AD5" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="AE5" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="AF5" s="31"/>
+      <c r="AG5" s="31"/>
+      <c r="AH5" s="31"/>
+      <c r="AI5" s="28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="22">
+        <v>108450068</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="23">
+        <v>26685</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="H6" s="22">
+        <v>22628427</v>
+      </c>
+      <c r="I6" s="22">
+        <v>83420020</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="K6" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="L6" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="M6" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="O6" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="R6" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="S6" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="T6" s="22"/>
+      <c r="U6" s="22">
+        <v>2005</v>
+      </c>
+      <c r="V6" s="33"/>
+      <c r="W6" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="X6" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="Y6" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z6" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="AA6" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB6" s="22"/>
+      <c r="AC6" s="22"/>
+      <c r="AD6" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="AE6" s="30"/>
+      <c r="AF6" s="22"/>
+      <c r="AG6" s="22"/>
+      <c r="AH6" s="22"/>
+      <c r="AI6" s="26" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{AA511A06-B3DE-4167-B031-82419FA2DEE4}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{5E9ED5D1-8591-433C-94F8-3DF1CE8D0412}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{EA2BCBF3-BFEB-488B-9D9B-E44B1AE76954}"/>
+    <hyperlink ref="G3" r:id="rId4" xr:uid="{A5FE723F-BD18-43AF-BFC3-ACD8CC293DC3}"/>
+    <hyperlink ref="F4" r:id="rId5" xr:uid="{D35C6B6E-BB57-457A-9FAF-DE322D408E25}"/>
+    <hyperlink ref="G4" r:id="rId6" xr:uid="{AADFD5D3-764D-420E-95BE-019BF2528CAE}"/>
+    <hyperlink ref="F5" r:id="rId7" xr:uid="{637C0C50-25F1-421F-B1BD-4D3FBDADA777}"/>
+    <hyperlink ref="G5" r:id="rId8" xr:uid="{7B8E8936-06E4-4F87-88D5-94A4A0AB3778}"/>
+    <hyperlink ref="F6" r:id="rId9" xr:uid="{B344B6F9-5E2B-4F25-9175-C0523199BB49}"/>
+    <hyperlink ref="G6" r:id="rId10" xr:uid="{0C066BD0-EFAB-4C2F-BDF6-8738D41B533D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId11"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EC084F-F78E-4A98-B67C-45E7481369F0}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>